<commit_message>
Added density values to data
</commit_message>
<xml_diff>
--- a/data/data_all.xlsx
+++ b/data/data_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagas\PycharmProjects\RaspberryPi_KI\eco_vision\interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagas\PycharmProjects\EcoVision\EcoVision\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E77F04-9A88-430F-9F61-78BBC8CFAFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E141A-E644-4173-A127-4F67352547EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>Foodstuff</t>
   </si>
@@ -180,6 +180,84 @@
   </si>
   <si>
     <t>Tomato</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>1.09</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.60</t>
   </si>
 </sst>
 </file>
@@ -281,7 +359,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,20 +642,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,500 +665,638 @@
       <c r="C1" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>0.3</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>0.7</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>1.6E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>0.6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>0.6</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3">
         <v>0.8</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="3">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>0.2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="3">
         <v>0.19500000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="3">
         <v>0.6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="3">
         <v>0.11899999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>0.45</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="3">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>0.3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="3">
         <v>0.3</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3">
         <v>0.2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="3">
         <v>1.8149999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="3">
         <v>0.1</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="3">
         <v>0.2</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="3">
         <v>0.56699999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="3">
         <v>0.2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <v>0.113</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.4</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="3">
         <v>0.22700000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="3">
         <v>0.2</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="3">
         <v>1.0209999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="3">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="3">
         <v>0.46</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="3">
         <v>4.2500000000000003E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="3">
         <v>0.88</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="3">
         <v>5.7000000000000002E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3">
         <v>0.17599999999999999</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="3">
         <v>0.45400000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="3">
         <v>0.4</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="3">
         <v>0.62350000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3">
         <v>3.47</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="3">
         <v>0.16800000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="3">
         <v>0.379</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="3">
         <v>1.2</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="3">
         <v>0.53900000000000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="3">
         <v>0.89</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="3">
         <v>0.33600000000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="3">
         <v>0.71</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="3">
         <v>2.04</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="3">
         <v>1.3</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="3">
         <v>0.22700000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="3">
         <v>0.2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="3">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="3">
         <v>0.3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="3">
         <v>0.13100000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="3">
         <v>4.4999999999999998E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="3">
         <v>0.2</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="3">
         <v>0.3</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="3">
         <v>0.17799999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="3">
         <v>0.4</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="3">
         <v>0.45400000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="3">
         <v>0.9</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="3">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="3">
         <v>0.88</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="3">
         <v>6.6000000000000003E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="3">
         <v>0.86</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="3">
         <v>0.28199999999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="3">
         <v>0.2</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="3">
         <v>0.21299999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="3">
         <v>0.2</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="3">
         <v>5.44</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="3">
         <v>0.2</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="3">
         <v>0.33</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="3">
         <v>5.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="3">
         <v>0.3</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="3">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="3">
         <v>0.8</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="3">
         <v>0.123</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B45" s="3">
         <v>0.05</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="3">
         <v>4.5350000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="3">
         <v>0.2</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="3">
         <v>0.19600000000000001</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>